<commit_message>
changing selenium java version 4.6.0
</commit_message>
<xml_diff>
--- a/src/main/java/com/tutorialsninja/qa/testdata/TutorialsNinjaTestData.xlsx
+++ b/src/main/java/com/tutorialsninja/qa/testdata/TutorialsNinjaTestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DHEERENDRA\git\TutorialsNinjaHybridFrameworkRepo\src\main\java\com\tutorialsninja\qa\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DHEERENDRA\git\TUTORIAL\src\main\java\com\tutorialsninja\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D7E77F-8C4A-463D-94AD-359E5917985E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA991204-17B0-4BBC-BB66-FBA1AAA6A94A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D7623641-1D76-4CA1-A366-04F62E4AA1D3}"/>
+    <workbookView xWindow="2205" yWindow="2205" windowWidth="15375" windowHeight="7875" xr2:uid="{D7623641-1D76-4CA1-A366-04F62E4AA1D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Email</t>
   </si>
@@ -34,18 +34,6 @@
   </si>
   <si>
     <t>dheeruvish1608@gmail.com</t>
-  </si>
-  <si>
-    <t>dheeruvish1609@gmail.com</t>
-  </si>
-  <si>
-    <t>dheeruvish1610@gmail.com</t>
-  </si>
-  <si>
-    <t>dheeruvish1611@gmail.com</t>
-  </si>
-  <si>
-    <t>dheeruvish1612@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -122,11 +110,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -444,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F41CE02-E721-4943-90D4-67B3987DFCAC}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,48 +454,12 @@
         <v>2</v>
       </c>
       <c r="B2" s="3">
-        <v>12345</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3">
-        <v>12345</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="3">
-        <v>12345</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="3">
-        <v>12345</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="5">
-        <v>12345</v>
+        <v>123456</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{60FEB029-EE5B-45F6-8DE6-F97638432156}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{72BF88CA-C10E-44B2-843E-4C6AE7E8AC53}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{702BBD34-2AA9-45FF-A042-39E3802F70A2}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{763DF6F9-29DA-4343-9537-64A58D88F596}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{C10292A5-BCCB-41EF-93FA-312DA3C07280}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{C10292A5-BCCB-41EF-93FA-312DA3C07280}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>